<commit_message>
Add production follow-up script and template for report generation
- Implemented `production_followup.py` to automate the creation of production reports based on a CSV input.
- Added functionality to select dates for report generation, defaulting to yesterday.
- Integrated Excel file handling using `openpyxl` to populate a template with production data.
- Created a new Excel template file for production follow-up.
</commit_message>
<xml_diff>
--- a/05. May/07-May-25.xlsx
+++ b/05. May/07-May-25.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1. Work\1. Daily\Production follow up\05. May\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7038E796-1388-4F16-8BA1-8D6717F91FBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48EED7F-7D75-41E6-B00D-0369CD11461E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -609,7 +609,7 @@
   <dimension ref="A1:X23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,8 +640,8 @@
         <v>1</v>
       </c>
       <c r="B2" s="5">
-        <f ca="1">TODAY() - 1</f>
-        <v>45784</v>
+        <f ca="1">TODAY() - 2</f>
+        <v>45785</v>
       </c>
     </row>
     <row r="3" spans="1:24" ht="76.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>